<commit_message>
master update for product and dial
</commit_message>
<xml_diff>
--- a/Documents/Ajit Bakery Masters.xlsx
+++ b/Documents/Ajit Bakery Masters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Product Master" sheetId="1" r:id="rId1"/>
@@ -540,12 +540,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Dhiraj" id="{646DCBC3-52B2-4DA5-B0C5-E6EAD1D4A601}" userId="Dhiraj" providerId="None"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,20 +857,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F1" dT="2025-03-06T09:05:53.93" personId="{646DCBC3-52B2-4DA5-B0C5-E6EAD1D4A601}" id="{99A30A22-6A9D-4DBB-8DF7-3929F6CED523}">
-    <text xml:space="preserve">Please add the size if found in circle then enter diamter(15cm) and if square enter (l*b) </text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1785,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>